<commit_message>
Added run script and hacked release schedule and other data files to make it run
</commit_message>
<xml_diff>
--- a/data/decc/data_release_schedule.xlsx
+++ b/data/decc/data_release_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/decc-archive/data/decc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE15CD3B-EB00-1648-8867-933ACAAED96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72384B69-EB6E-9349-B8F7-AF3AA3E0614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="500" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="11160" yWindow="500" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="GCMD" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -222,14 +222,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +263,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +369,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5DB9A0-5433-FF47-BABC-7C9213421903}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,6 +703,12 @@
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -774,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E362F148-5D79-214D-93BA-FD6AF7AFDC2B}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -834,10 +836,16 @@
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>